<commit_message>
Weekly update Eclipse 26/2/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J531"/>
+  <dimension ref="A1:J532"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17322,31 +17322,63 @@
         <v>45705</v>
       </c>
       <c r="B531">
-        <v>2.137790446805443</v>
+        <v>2.152281426695374</v>
       </c>
       <c r="C531">
-        <v>0.490561402051162</v>
+        <v>0.490398757795606</v>
       </c>
       <c r="D531">
-        <v>2.395305803452226</v>
+        <v>2.403120917869384</v>
       </c>
       <c r="E531">
-        <v>54.84535225</v>
+        <v>55.07346588</v>
       </c>
       <c r="F531">
-        <v>59.75687097119386</v>
+        <v>60.67013541213771</v>
       </c>
       <c r="G531">
-        <v>1.048905426508895</v>
+        <v>1.02066231212559</v>
       </c>
       <c r="H531">
-        <v>0.4970814768624932</v>
+        <v>0.2961797266078481</v>
       </c>
       <c r="I531">
         <v>0.6774045825004578</v>
       </c>
       <c r="J531">
-        <v>95337.62</v>
+        <v>96091.63297749851</v>
+      </c>
+    </row>
+    <row r="532" spans="1:10">
+      <c r="A532" s="2">
+        <v>45712</v>
+      </c>
+      <c r="B532">
+        <v>1.980493346251423</v>
+      </c>
+      <c r="C532">
+        <v>0.4851908573271597</v>
+      </c>
+      <c r="D532">
+        <v>2.067286854478257</v>
+      </c>
+      <c r="E532">
+        <v>53.01406224</v>
+      </c>
+      <c r="F532">
+        <v>52.38490078887447</v>
+      </c>
+      <c r="G532">
+        <v>1.017658429823554</v>
+      </c>
+      <c r="H532">
+        <v>-0.2167236233498793</v>
+      </c>
+      <c r="I532">
+        <v>0.6819115281105042</v>
+      </c>
+      <c r="J532">
+        <v>88845.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly updat eclipse 3/5
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J532"/>
+  <dimension ref="A1:J533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17354,31 +17354,63 @@
         <v>45712</v>
       </c>
       <c r="B532">
-        <v>1.980493346251423</v>
+        <v>2.09749010064619</v>
       </c>
       <c r="C532">
-        <v>0.4851908573271597</v>
+        <v>0.4840445794792705</v>
       </c>
       <c r="D532">
-        <v>2.067286854478257</v>
+        <v>2.307412762143986</v>
       </c>
       <c r="E532">
-        <v>53.01406224</v>
+        <v>49.63466733</v>
       </c>
       <c r="F532">
-        <v>52.38490078887447</v>
+        <v>58.42113049885942</v>
       </c>
       <c r="G532">
         <v>1.017658429823554</v>
       </c>
       <c r="H532">
-        <v>-0.2167236233498793</v>
+        <v>1.212509725306887</v>
       </c>
       <c r="I532">
         <v>0.6819115281105042</v>
       </c>
       <c r="J532">
-        <v>88845.87</v>
+        <v>94328.00944447691</v>
+      </c>
+    </row>
+    <row r="533" spans="1:10">
+      <c r="A533" s="2">
+        <v>45719</v>
+      </c>
+      <c r="B533">
+        <v>1.942984320442183</v>
+      </c>
+      <c r="C533">
+        <v>0.4807847074602101</v>
+      </c>
+      <c r="D533">
+        <v>1.989049508589191</v>
+      </c>
+      <c r="E533">
+        <v>49.71989554</v>
+      </c>
+      <c r="F533">
+        <v>50.69942998149145</v>
+      </c>
+      <c r="G533">
+        <v>1.015097711010136</v>
+      </c>
+      <c r="H533">
+        <v>-0.9207002237236028</v>
+      </c>
+      <c r="I533">
+        <v>0.6878000497817993</v>
+      </c>
+      <c r="J533">
+        <v>87599.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update Eclipse 10/03/2025
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J533"/>
+  <dimension ref="A1:J534"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17386,31 +17386,63 @@
         <v>45719</v>
       </c>
       <c r="B533">
-        <v>1.942984320442183</v>
+        <v>1.785116575029412</v>
       </c>
       <c r="C533">
-        <v>0.4807847074602101</v>
+        <v>0.4822126256051544</v>
       </c>
       <c r="D533">
-        <v>1.989049508589191</v>
+        <v>1.675130573751481</v>
       </c>
       <c r="E533">
-        <v>49.71989554</v>
+        <v>49.58605341</v>
       </c>
       <c r="F533">
-        <v>50.69942998149145</v>
+        <v>44.60781212959165</v>
       </c>
       <c r="G533">
-        <v>1.015097711010136</v>
+        <v>1.02748250590624</v>
       </c>
       <c r="H533">
-        <v>-0.9207002237236028</v>
+        <v>-0.4586943466390769</v>
       </c>
       <c r="I533">
         <v>0.6878000497817993</v>
       </c>
       <c r="J533">
-        <v>87599.55</v>
+        <v>80647.7964108709</v>
+      </c>
+    </row>
+    <row r="534" spans="1:10">
+      <c r="A534" s="2">
+        <v>45726</v>
+      </c>
+      <c r="B534">
+        <v>1.832323919611125</v>
+      </c>
+      <c r="C534">
+        <v>0.4802972352685188</v>
+      </c>
+      <c r="D534">
+        <v>1.76772495165094</v>
+      </c>
+      <c r="E534">
+        <v>45.41281397</v>
+      </c>
+      <c r="F534">
+        <v>47.04096332102084</v>
+      </c>
+      <c r="G534">
+        <v>1.023464311052906</v>
+      </c>
+      <c r="H534">
+        <v>0.1979928135648068</v>
+      </c>
+      <c r="I534">
+        <v>0.6864444017410278</v>
+      </c>
+      <c r="J534">
+        <v>83116.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 3/19/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J534"/>
+  <dimension ref="A1:J535"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17418,31 +17418,63 @@
         <v>45726</v>
       </c>
       <c r="B534">
-        <v>1.832323919611125</v>
+        <v>1.815928460182456</v>
       </c>
       <c r="C534">
-        <v>0.4802972352685188</v>
+        <v>0.4804242620176978</v>
       </c>
       <c r="D534">
-        <v>1.76772495165094</v>
+        <v>1.745643531111315</v>
       </c>
       <c r="E534">
-        <v>45.41281397</v>
+        <v>48.40436123</v>
       </c>
       <c r="F534">
-        <v>47.04096332102084</v>
+        <v>46.44622501294415</v>
       </c>
       <c r="G534">
         <v>1.023464311052906</v>
       </c>
       <c r="H534">
-        <v>0.1979928135648068</v>
+        <v>0.07498102013752117</v>
       </c>
       <c r="I534">
         <v>0.6864444017410278</v>
       </c>
       <c r="J534">
-        <v>83116.16</v>
+        <v>82492.1028287551</v>
+      </c>
+    </row>
+    <row r="535" spans="1:10">
+      <c r="A535" s="2">
+        <v>45733</v>
+      </c>
+      <c r="B535">
+        <v>1.812914666627164</v>
+      </c>
+      <c r="C535">
+        <v>0.4794602211472156</v>
+      </c>
+      <c r="D535">
+        <v>1.752638144396374</v>
+      </c>
+      <c r="E535">
+        <v>48.17859296</v>
+      </c>
+      <c r="F535">
+        <v>46.40040700203526</v>
+      </c>
+      <c r="G535">
+        <v>1.020045074635872</v>
+      </c>
+      <c r="H535">
+        <v>-0.04155288231265652</v>
+      </c>
+      <c r="I535">
+        <v>0.681629478931427</v>
+      </c>
+      <c r="J535">
+        <v>82441.14999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 3/26/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J535"/>
+  <dimension ref="A1:J536"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17450,31 +17450,63 @@
         <v>45733</v>
       </c>
       <c r="B535">
-        <v>1.812914666627164</v>
+        <v>1.882119349760018</v>
       </c>
       <c r="C535">
-        <v>0.4794602211472156</v>
+        <v>0.4787920636151367</v>
       </c>
       <c r="D535">
-        <v>1.752638144396374</v>
+        <v>1.87808353230159</v>
       </c>
       <c r="E535">
-        <v>48.17859296</v>
+        <v>48.06036485</v>
       </c>
       <c r="F535">
-        <v>46.40040700203526</v>
+        <v>49.63663426698965</v>
       </c>
       <c r="G535">
-        <v>1.020045074635872</v>
+        <v>1.032513244813934</v>
       </c>
       <c r="H535">
-        <v>-0.04155288231265652</v>
+        <v>0.5764913929558357</v>
       </c>
       <c r="I535">
         <v>0.681629478931427</v>
       </c>
       <c r="J535">
-        <v>82441.14999999999</v>
+        <v>85760.8814506137</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10">
+      <c r="A536" s="2">
+        <v>45740</v>
+      </c>
+      <c r="B536">
+        <v>1.917293835612691</v>
+      </c>
+      <c r="C536">
+        <v>0.4797430502987418</v>
+      </c>
+      <c r="D536">
+        <v>1.948745990405471</v>
+      </c>
+      <c r="E536">
+        <v>50.10023951</v>
+      </c>
+      <c r="F536">
+        <v>51.27494120578657</v>
+      </c>
+      <c r="G536">
+        <v>1.027739651827525</v>
+      </c>
+      <c r="H536">
+        <v>0.4142038584296293</v>
+      </c>
+      <c r="I536">
+        <v>0.6774072647094727</v>
+      </c>
+      <c r="J536">
+        <v>87474</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 3/31/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J536"/>
+  <dimension ref="A1:J537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17482,31 +17482,63 @@
         <v>45740</v>
       </c>
       <c r="B536">
-        <v>1.917293835612691</v>
+        <v>1.80175842007386</v>
       </c>
       <c r="C536">
-        <v>0.4797430502987418</v>
+        <v>0.4808010010192146</v>
       </c>
       <c r="D536">
-        <v>1.948745990405471</v>
+        <v>1.706697418545975</v>
       </c>
       <c r="E536">
-        <v>50.10023951</v>
+        <v>46.84289835</v>
       </c>
       <c r="F536">
-        <v>51.27494120578657</v>
+        <v>46.40818057293777</v>
       </c>
       <c r="G536">
         <v>1.027739651827525</v>
       </c>
       <c r="H536">
-        <v>0.4142038584296293</v>
+        <v>-0.4579008609819635</v>
       </c>
       <c r="I536">
         <v>0.6774072647094727</v>
       </c>
       <c r="J536">
-        <v>87474</v>
+        <v>82216.4666765049</v>
+      </c>
+    </row>
+    <row r="537" spans="1:10">
+      <c r="A537" s="2">
+        <v>45747</v>
+      </c>
+      <c r="B537">
+        <v>1.866632756412493</v>
+      </c>
+      <c r="C537">
+        <v>0.4845703712335291</v>
+      </c>
+      <c r="D537">
+        <v>1.838663445197967</v>
+      </c>
+      <c r="E537">
+        <v>47.05625261</v>
+      </c>
+      <c r="F537">
+        <v>49.46836317119275</v>
+      </c>
+      <c r="G537">
+        <v>1.023682993282466</v>
+      </c>
+      <c r="H537">
+        <v>0.3327304826337363</v>
+      </c>
+      <c r="I537">
+        <v>0.6716356873512268</v>
+      </c>
+      <c r="J537">
+        <v>85280.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 4/9/2025
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J537"/>
+  <dimension ref="A1:J538"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17514,31 +17514,63 @@
         <v>45747</v>
       </c>
       <c r="B537">
-        <v>1.866632756412493</v>
+        <v>1.6985183741486</v>
       </c>
       <c r="C537">
-        <v>0.4845703712335291</v>
+        <v>0.486073864997257</v>
       </c>
       <c r="D537">
-        <v>1.838663445197967</v>
+        <v>1.50633876854923</v>
       </c>
       <c r="E537">
-        <v>47.05625261</v>
+        <v>47.18767409</v>
       </c>
       <c r="F537">
-        <v>49.46836317119275</v>
+        <v>42.79885802011866</v>
       </c>
       <c r="G537">
-        <v>1.023682993282466</v>
+        <v>1.08263967419379</v>
       </c>
       <c r="H537">
-        <v>0.3327304826337363</v>
+        <v>-0.417202074118439</v>
       </c>
       <c r="I537">
         <v>0.6716356873512268</v>
       </c>
       <c r="J537">
-        <v>85280.91</v>
+        <v>77949.0884926943</v>
+      </c>
+    </row>
+    <row r="538" spans="1:10">
+      <c r="A538" s="2">
+        <v>45754</v>
+      </c>
+      <c r="B538">
+        <v>1.672745636546524</v>
+      </c>
+      <c r="C538">
+        <v>0.4936289872506107</v>
+      </c>
+      <c r="D538">
+        <v>1.435469552700401</v>
+      </c>
+      <c r="E538">
+        <v>44.79094424</v>
+      </c>
+      <c r="F538">
+        <v>42.0064765051406</v>
+      </c>
+      <c r="G538">
+        <v>1.070007520920395</v>
+      </c>
+      <c r="H538">
+        <v>0.06774560119782169</v>
+      </c>
+      <c r="I538">
+        <v>0.6611138582229614</v>
+      </c>
+      <c r="J538">
+        <v>76988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 4/16/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J538"/>
+  <dimension ref="A1:J539"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17546,31 +17546,63 @@
         <v>45754</v>
       </c>
       <c r="B538">
-        <v>1.672745636546524</v>
+        <v>1.808642182982328</v>
       </c>
       <c r="C538">
-        <v>0.4936289872506107</v>
+        <v>0.4922369844524472</v>
       </c>
       <c r="D538">
-        <v>1.435469552700401</v>
+        <v>1.740983508531215</v>
       </c>
       <c r="E538">
-        <v>44.79094424</v>
+        <v>48.6275228</v>
       </c>
       <c r="F538">
-        <v>42.0064765051406</v>
+        <v>48.48142427175795</v>
       </c>
       <c r="G538">
         <v>1.070007520920395</v>
       </c>
       <c r="H538">
-        <v>0.06774560119782169</v>
+        <v>1.054389511503784</v>
       </c>
       <c r="I538">
         <v>0.6611138582229614</v>
       </c>
       <c r="J538">
-        <v>76988</v>
+        <v>83568.9544360023</v>
+      </c>
+    </row>
+    <row r="539" spans="1:10">
+      <c r="A539" s="2">
+        <v>45761</v>
+      </c>
+      <c r="B539">
+        <v>1.811774109552587</v>
+      </c>
+      <c r="C539">
+        <v>0.4985081194509074</v>
+      </c>
+      <c r="D539">
+        <v>1.745135402803062</v>
+      </c>
+      <c r="E539">
+        <v>48.11680039</v>
+      </c>
+      <c r="F539">
+        <v>48.80952875079814</v>
+      </c>
+      <c r="G539">
+        <v>1.059412260068952</v>
+      </c>
+      <c r="H539">
+        <v>-0.8543325491649156</v>
+      </c>
+      <c r="I539">
+        <v>0.6502456665039062</v>
+      </c>
+      <c r="J539">
+        <v>83905.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 4/23
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J539"/>
+  <dimension ref="A1:J540"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17578,31 +17578,63 @@
         <v>45761</v>
       </c>
       <c r="B539">
-        <v>1.811774109552587</v>
+        <v>1.833631359001424</v>
       </c>
       <c r="C539">
-        <v>0.4985081194509074</v>
+        <v>0.4982502695345901</v>
       </c>
       <c r="D539">
-        <v>1.745135402803062</v>
+        <v>1.802432891118666</v>
       </c>
       <c r="E539">
-        <v>48.11680039</v>
+        <v>48.6653269</v>
       </c>
       <c r="F539">
-        <v>48.80952875079814</v>
+        <v>49.94210161711194</v>
       </c>
       <c r="G539">
-        <v>1.059412260068952</v>
+        <v>1.072160484448199</v>
       </c>
       <c r="H539">
-        <v>-0.8543325491649156</v>
+        <v>0.362877749727164</v>
       </c>
       <c r="I539">
         <v>0.6502456665039062</v>
       </c>
       <c r="J539">
-        <v>83905.64</v>
+        <v>85101.74615458791</v>
+      </c>
+    </row>
+    <row r="540" spans="1:10">
+      <c r="A540" s="2">
+        <v>45768</v>
+      </c>
+      <c r="B540">
+        <v>2.005412215255971</v>
+      </c>
+      <c r="C540">
+        <v>0.5035851865684796</v>
+      </c>
+      <c r="D540">
+        <v>2.161380194536735</v>
+      </c>
+      <c r="E540">
+        <v>49.65986338</v>
+      </c>
+      <c r="F540">
+        <v>56.93292817063122</v>
+      </c>
+      <c r="G540">
+        <v>1.061220741192354</v>
+      </c>
+      <c r="H540">
+        <v>1.558717387382536</v>
+      </c>
+      <c r="I540">
+        <v>0.6386415362358093</v>
+      </c>
+      <c r="J540">
+        <v>93250.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 30/4/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J540"/>
+  <dimension ref="A1:J541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17610,31 +17610,63 @@
         <v>45768</v>
       </c>
       <c r="B540">
-        <v>2.005412215255971</v>
+        <v>2.007064223561584</v>
       </c>
       <c r="C540">
-        <v>0.5035851865684796</v>
+        <v>0.5034619422573574</v>
       </c>
       <c r="D540">
-        <v>2.161380194536735</v>
+        <v>2.145063430539812</v>
       </c>
       <c r="E540">
-        <v>49.65986338</v>
+        <v>53.02736129</v>
       </c>
       <c r="F540">
-        <v>56.93292817063122</v>
+        <v>57.34405092703624</v>
       </c>
       <c r="G540">
         <v>1.061220741192354</v>
       </c>
       <c r="H540">
-        <v>1.558717387382536</v>
+        <v>0.7700683636846728</v>
       </c>
       <c r="I540">
         <v>0.6386415362358093</v>
       </c>
       <c r="J540">
-        <v>93250.5</v>
+        <v>93812.876534775</v>
+      </c>
+    </row>
+    <row r="541" spans="1:10">
+      <c r="A541" s="2">
+        <v>45775</v>
+      </c>
+      <c r="B541">
+        <v>2.01220298028551</v>
+      </c>
+      <c r="C541">
+        <v>0.5094351357331968</v>
+      </c>
+      <c r="D541">
+        <v>2.149827372442422</v>
+      </c>
+      <c r="E541">
+        <v>52.9957549</v>
+      </c>
+      <c r="F541">
+        <v>57.93759369932081</v>
+      </c>
+      <c r="G541">
+        <v>1.052019963773586</v>
+      </c>
+      <c r="H541">
+        <v>2.216421728980222</v>
+      </c>
+      <c r="I541">
+        <v>0.6292807459831238</v>
+      </c>
+      <c r="J541">
+        <v>94584.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 5/7/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J541"/>
+  <dimension ref="A1:J542"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17642,31 +17642,63 @@
         <v>45775</v>
       </c>
       <c r="B541">
-        <v>2.01220298028551</v>
+        <v>2.00308044182545</v>
       </c>
       <c r="C541">
-        <v>0.5094351357331968</v>
+        <v>0.5094814150464051</v>
       </c>
       <c r="D541">
-        <v>2.149827372442422</v>
+        <v>2.140586316360153</v>
       </c>
       <c r="E541">
-        <v>52.9957549</v>
+        <v>53.61823884</v>
       </c>
       <c r="F541">
-        <v>57.93759369932081</v>
+        <v>57.78004769213506</v>
       </c>
       <c r="G541">
-        <v>1.052019963773586</v>
+        <v>1.021997222157899</v>
       </c>
       <c r="H541">
-        <v>2.216421728980222</v>
+        <v>0.1713414492450882</v>
       </c>
       <c r="I541">
         <v>0.6292807459831238</v>
       </c>
       <c r="J541">
-        <v>94584.8</v>
+        <v>94377.78991963759</v>
+      </c>
+    </row>
+    <row r="542" spans="1:10">
+      <c r="A542" s="2">
+        <v>45782</v>
+      </c>
+      <c r="B542">
+        <v>1.993695139660456</v>
+      </c>
+      <c r="C542">
+        <v>0.512903535607143</v>
+      </c>
+      <c r="D542">
+        <v>2.229784229026972</v>
+      </c>
+      <c r="E542">
+        <v>52.74870033</v>
+      </c>
+      <c r="F542">
+        <v>58.13837013170215</v>
+      </c>
+      <c r="G542">
+        <v>1.01879569711747</v>
+      </c>
+      <c r="H542">
+        <v>1.89837261116419</v>
+      </c>
+      <c r="I542">
+        <v>0.6225997805595398</v>
+      </c>
+      <c r="J542">
+        <v>94817.08</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 5/14/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J542"/>
+  <dimension ref="A1:J543"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17674,31 +17674,63 @@
         <v>45782</v>
       </c>
       <c r="B542">
-        <v>1.993695139660456</v>
+        <v>2.179648447758372</v>
       </c>
       <c r="C542">
-        <v>0.512903535607143</v>
+        <v>0.5108484896487172</v>
       </c>
       <c r="D542">
-        <v>2.229784229026972</v>
+        <v>2.512200364464867</v>
       </c>
       <c r="E542">
-        <v>52.74870033</v>
+        <v>56.4754816</v>
       </c>
       <c r="F542">
-        <v>58.13837013170215</v>
+        <v>64.43217137419421</v>
       </c>
       <c r="G542">
         <v>1.01879569711747</v>
       </c>
       <c r="H542">
-        <v>1.89837261116419</v>
+        <v>1.120049613003382</v>
       </c>
       <c r="I542">
         <v>0.6225997805595398</v>
       </c>
       <c r="J542">
-        <v>94817.08</v>
+        <v>103976.137798948</v>
+      </c>
+    </row>
+    <row r="543" spans="1:10">
+      <c r="A543" s="2">
+        <v>45789</v>
+      </c>
+      <c r="B543">
+        <v>2.174439356243377</v>
+      </c>
+      <c r="C543">
+        <v>0.5117533967000821</v>
+      </c>
+      <c r="D543">
+        <v>2.508154674679554</v>
+      </c>
+      <c r="E543">
+        <v>55.71173169</v>
+      </c>
+      <c r="F543">
+        <v>64.71225868421709</v>
+      </c>
+      <c r="G543">
+        <v>1.016067454812958</v>
+      </c>
+      <c r="H543">
+        <v>3.217227839943848</v>
+      </c>
+      <c r="I543">
+        <v>0.6211040616035461</v>
+      </c>
+      <c r="J543">
+        <v>104425.13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly update eclipse 5/28/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J544"/>
+  <dimension ref="A1:J545"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -16688,7 +16688,7 @@
         <v>0.6330298148749738</v>
       </c>
       <c r="D511">
-        <v>1.695086696571917</v>
+        <v>1.696164974940352</v>
       </c>
       <c r="E511">
         <v>48.37127543</v>
@@ -16720,7 +16720,7 @@
         <v>0.63939715874584</v>
       </c>
       <c r="D512">
-        <v>1.664324959301048</v>
+        <v>1.665551996557877</v>
       </c>
       <c r="E512">
         <v>48.79273292</v>
@@ -16735,7 +16735,7 @@
         <v>0.794711395600034</v>
       </c>
       <c r="I512">
-        <v>0.4624601900577545</v>
+        <v>0.4624643623828888</v>
       </c>
       <c r="J512">
         <v>62759.431113384</v>
@@ -16752,7 +16752,7 @@
         <v>0.6424155030609533</v>
       </c>
       <c r="D513">
-        <v>1.977192857158895</v>
+        <v>1.978709591462637</v>
       </c>
       <c r="E513">
         <v>52.07061351</v>
@@ -16767,7 +16767,7 @@
         <v>5.973047604075576</v>
       </c>
       <c r="I513">
-        <v>0.4666055142879486</v>
+        <v>0.4666163325309753</v>
       </c>
       <c r="J513">
         <v>69012.35320894211</v>
@@ -16784,7 +16784,7 @@
         <v>0.6465871895242613</v>
       </c>
       <c r="D514">
-        <v>1.901742891082644</v>
+        <v>1.903324545069853</v>
       </c>
       <c r="E514">
         <v>51.03196562</v>
@@ -16799,7 +16799,7 @@
         <v>1.094576386141322</v>
       </c>
       <c r="I514">
-        <v>0.4769414961338043</v>
+        <v>0.4769619107246399</v>
       </c>
       <c r="J514">
         <v>68000.1475008767</v>
@@ -16816,7 +16816,7 @@
         <v>0.6483252865846113</v>
       </c>
       <c r="D515">
-        <v>1.916641925929204</v>
+        <v>1.918084078079499</v>
       </c>
       <c r="E515">
         <v>51.76475474</v>
@@ -16831,7 +16831,7 @@
         <v>0.3970273283649517</v>
       </c>
       <c r="I515">
-        <v>0.4838529527187347</v>
+        <v>0.4838846623897552</v>
       </c>
       <c r="J515">
         <v>68742.7546227352</v>
@@ -16848,7 +16848,7 @@
         <v>0.642922359204719</v>
       </c>
       <c r="D516">
-        <v>2.497704217903252</v>
+        <v>2.501440986327097</v>
       </c>
       <c r="E516">
         <v>55.96035811</v>
@@ -16863,7 +16863,7 @@
         <v>2.745434731379093</v>
       </c>
       <c r="I516">
-        <v>0.4894328415393829</v>
+        <v>0.489477127790451</v>
       </c>
       <c r="J516">
         <v>80409.28656662771</v>
@@ -16880,7 +16880,7 @@
         <v>0.6336821575168828</v>
       </c>
       <c r="D517">
-        <v>2.900783691959819</v>
+        <v>2.905218012358775</v>
       </c>
       <c r="E517">
         <v>61.08620585</v>
@@ -16895,7 +16895,7 @@
         <v>1.792304909417264</v>
       </c>
       <c r="I517">
-        <v>0.5007900595664978</v>
+        <v>0.5008559226989746</v>
       </c>
       <c r="J517">
         <v>89732.97042928109</v>
@@ -16912,7 +16912,7 @@
         <v>0.6187644675843351</v>
       </c>
       <c r="D518">
-        <v>3.214332093114661</v>
+        <v>3.219467902151182</v>
       </c>
       <c r="E518">
         <v>62.61633967</v>
@@ -16927,7 +16927,7 @@
         <v>2.816405718103709</v>
       </c>
       <c r="I518">
-        <v>0.5180327296257019</v>
+        <v>0.5181275010108948</v>
       </c>
       <c r="J518">
         <v>97980.2082819988</v>
@@ -16944,7 +16944,7 @@
         <v>0.6070289417996042</v>
       </c>
       <c r="D519">
-        <v>3.120391843799167</v>
+        <v>3.125546196159932</v>
       </c>
       <c r="E519">
         <v>61.50908662</v>
@@ -16959,7 +16959,7 @@
         <v>1.97434518729358</v>
       </c>
       <c r="I519">
-        <v>0.5399569869041443</v>
+        <v>0.5400869250297546</v>
       </c>
       <c r="J519">
         <v>97469.60445295151</v>
@@ -16976,7 +16976,7 @@
         <v>0.5972935892914361</v>
       </c>
       <c r="D520">
-        <v>3.194460751785761</v>
+        <v>3.199803954257344</v>
       </c>
       <c r="E520">
         <v>61.64293554</v>
@@ -16991,7 +16991,7 @@
         <v>1.771398933059798</v>
       </c>
       <c r="I520">
-        <v>0.5623756647109985</v>
+        <v>0.5625441074371338</v>
       </c>
       <c r="J520">
         <v>100798.98356429</v>
@@ -17008,7 +17008,7 @@
         <v>0.586097838206267</v>
       </c>
       <c r="D521">
-        <v>3.298694534251457</v>
+        <v>3.305243572689947</v>
       </c>
       <c r="E521">
         <v>61.32892133</v>
@@ -17023,7 +17023,7 @@
         <v>3.267794682905678</v>
       </c>
       <c r="I521">
-        <v>0.5853249430656433</v>
+        <v>0.5855334997177124</v>
       </c>
       <c r="J521">
         <v>104551.367141146</v>
@@ -17040,7 +17040,7 @@
         <v>0.5740518574020853</v>
       </c>
       <c r="D522">
-        <v>2.740898093106181</v>
+        <v>2.744941014157402</v>
       </c>
       <c r="E522">
         <v>58.74535966</v>
@@ -17055,7 +17055,7 @@
         <v>6.738133550749792</v>
       </c>
       <c r="I522">
-        <v>0.6082763671875</v>
+        <v>0.6085300445556641</v>
       </c>
       <c r="J522">
         <v>95149.10582524841</v>
@@ -17072,7 +17072,7 @@
         <v>0.564106006837494</v>
       </c>
       <c r="D523">
-        <v>2.601696824493982</v>
+        <v>2.605215748062194</v>
       </c>
       <c r="E523">
         <v>57.24026093</v>
@@ -17087,7 +17087,7 @@
         <v>1.690977793454818</v>
       </c>
       <c r="I523">
-        <v>0.623753547668457</v>
+        <v>0.6240490674972534</v>
       </c>
       <c r="J523">
         <v>93457.57832028061</v>
@@ -17104,7 +17104,7 @@
         <v>0.5527709916209589</v>
       </c>
       <c r="D524">
-        <v>2.796260968720684</v>
+        <v>2.800969984942633</v>
       </c>
       <c r="E524">
         <v>58.14427333</v>
@@ -17119,7 +17119,7 @@
         <v>0.7210626257030839</v>
       </c>
       <c r="I524">
-        <v>0.6320773363113403</v>
+        <v>0.6324124336242676</v>
       </c>
       <c r="J524">
         <v>98414.81209643481</v>
@@ -17136,7 +17136,7 @@
         <v>0.5445277199826385</v>
       </c>
       <c r="D525">
-        <v>2.561536949017885</v>
+        <v>2.564996839721336</v>
       </c>
       <c r="E525">
         <v>56.26685989</v>
@@ -17151,7 +17151,7 @@
         <v>0.6197147672702075</v>
       </c>
       <c r="I525">
-        <v>0.6392703652381897</v>
+        <v>0.6396464705467224</v>
       </c>
       <c r="J525">
         <v>94353.77525862071</v>
@@ -17168,7 +17168,7 @@
         <v>0.5326133186424523</v>
       </c>
       <c r="D526">
-        <v>2.827033157625898</v>
+        <v>2.831601244616424</v>
       </c>
       <c r="E526">
         <v>58.51780586</v>
@@ -17183,7 +17183,7 @@
         <v>1.260794721631919</v>
       </c>
       <c r="I526">
-        <v>0.643413782119751</v>
+        <v>0.6438268423080444</v>
       </c>
       <c r="J526">
         <v>100954.572281999</v>
@@ -17200,7 +17200,7 @@
         <v>0.5201771747869814</v>
       </c>
       <c r="D527">
-        <v>2.853538897002827</v>
+        <v>2.857948528935437</v>
       </c>
       <c r="E527">
         <v>59.54210498</v>
@@ -17215,7 +17215,7 @@
         <v>0.8429865736807596</v>
       </c>
       <c r="I527">
-        <v>0.6506919860839844</v>
+        <v>0.6511408686637878</v>
       </c>
       <c r="J527">
         <v>102833.369273232</v>
@@ -17232,7 +17232,7 @@
         <v>0.5108436718503794</v>
       </c>
       <c r="D528">
-        <v>2.559692570813155</v>
+        <v>2.563515279422086</v>
       </c>
       <c r="E528">
         <v>57.46529285</v>
@@ -17247,7 +17247,7 @@
         <v>0.08790635023872007</v>
       </c>
       <c r="I528">
-        <v>0.6595891118049622</v>
+        <v>0.6600708365440369</v>
       </c>
       <c r="J528">
         <v>97424.78090005839</v>
@@ -17264,7 +17264,7 @@
         <v>0.503351974340427</v>
       </c>
       <c r="D529">
-        <v>2.467318465017778</v>
+        <v>2.470558777330556</v>
       </c>
       <c r="E529">
         <v>55.27625851</v>
@@ -17279,7 +17279,7 @@
         <v>3.623512206270152</v>
       </c>
       <c r="I529">
-        <v>0.6660023927688599</v>
+        <v>0.6665138006210327</v>
       </c>
       <c r="J529">
         <v>96309.7532405026</v>
@@ -17296,7 +17296,7 @@
         <v>0.4969347910321221</v>
       </c>
       <c r="D530">
-        <v>2.43314254816511</v>
+        <v>2.436138977448592</v>
       </c>
       <c r="E530">
         <v>55.58595516</v>
@@ -17311,7 +17311,7 @@
         <v>0.2087972792547355</v>
       </c>
       <c r="I530">
-        <v>0.6733283400535583</v>
+        <v>0.6738649010658264</v>
       </c>
       <c r="J530">
         <v>96182.2661706604</v>
@@ -17328,7 +17328,7 @@
         <v>0.490398757795606</v>
       </c>
       <c r="D531">
-        <v>2.403120917869384</v>
+        <v>2.405721974748321</v>
       </c>
       <c r="E531">
         <v>55.07346588</v>
@@ -17343,7 +17343,7 @@
         <v>0.2961797266078481</v>
       </c>
       <c r="I531">
-        <v>0.6774045825004578</v>
+        <v>0.677964985370636</v>
       </c>
       <c r="J531">
         <v>96091.63297749851</v>
@@ -17360,7 +17360,7 @@
         <v>0.4840445794792705</v>
       </c>
       <c r="D532">
-        <v>2.307412762143986</v>
+        <v>2.309496889533705</v>
       </c>
       <c r="E532">
         <v>49.63466733</v>
@@ -17375,7 +17375,7 @@
         <v>1.212509725306887</v>
       </c>
       <c r="I532">
-        <v>0.6819115281105042</v>
+        <v>0.6824901103973389</v>
       </c>
       <c r="J532">
         <v>94328.00944447691</v>
@@ -17392,7 +17392,7 @@
         <v>0.4822126256051544</v>
       </c>
       <c r="D533">
-        <v>1.675130573751481</v>
+        <v>1.676299684046415</v>
       </c>
       <c r="E533">
         <v>49.58605341</v>
@@ -17407,7 +17407,7 @@
         <v>-0.4586943466390769</v>
       </c>
       <c r="I533">
-        <v>0.6878000497817993</v>
+        <v>0.68839031457901</v>
       </c>
       <c r="J533">
         <v>80647.7964108709</v>
@@ -17424,7 +17424,7 @@
         <v>0.4804242620176978</v>
       </c>
       <c r="D534">
-        <v>1.745643531111315</v>
+        <v>1.747061705502933</v>
       </c>
       <c r="E534">
         <v>48.40436123</v>
@@ -17439,7 +17439,7 @@
         <v>0.07498102013752117</v>
       </c>
       <c r="I534">
-        <v>0.6864444017410278</v>
+        <v>0.6870439052581787</v>
       </c>
       <c r="J534">
         <v>82492.1028287551</v>
@@ -17456,7 +17456,7 @@
         <v>0.4787920636151367</v>
       </c>
       <c r="D535">
-        <v>1.87808353230159</v>
+        <v>1.879747782964211</v>
       </c>
       <c r="E535">
         <v>48.06036485</v>
@@ -17471,7 +17471,7 @@
         <v>0.5764913929558357</v>
       </c>
       <c r="I535">
-        <v>0.681629478931427</v>
+        <v>0.6822359561920166</v>
       </c>
       <c r="J535">
         <v>85760.8814506137</v>
@@ -17488,7 +17488,7 @@
         <v>0.4808010010192146</v>
       </c>
       <c r="D536">
-        <v>1.706697418545975</v>
+        <v>1.707971996714991</v>
       </c>
       <c r="E536">
         <v>46.84289835</v>
@@ -17503,7 +17503,7 @@
         <v>-0.4579008609819635</v>
       </c>
       <c r="I536">
-        <v>0.6774072647094727</v>
+        <v>0.6780171394348145</v>
       </c>
       <c r="J536">
         <v>82216.4666765049</v>
@@ -17520,7 +17520,7 @@
         <v>0.486073864997257</v>
       </c>
       <c r="D537">
-        <v>1.50633876854923</v>
+        <v>1.507336841296794</v>
       </c>
       <c r="E537">
         <v>47.18767409</v>
@@ -17535,7 +17535,7 @@
         <v>-0.417202074118439</v>
       </c>
       <c r="I537">
-        <v>0.6716356873512268</v>
+        <v>0.6722449660301208</v>
       </c>
       <c r="J537">
         <v>77949.0884926943</v>
@@ -17552,7 +17552,7 @@
         <v>0.4922369844524472</v>
       </c>
       <c r="D538">
-        <v>1.740983508531215</v>
+        <v>1.742335714943108</v>
       </c>
       <c r="E538">
         <v>48.6275228</v>
@@ -17567,7 +17567,7 @@
         <v>1.054389511503784</v>
       </c>
       <c r="I538">
-        <v>0.6611138582229614</v>
+        <v>0.6617199778556824</v>
       </c>
       <c r="J538">
         <v>83568.9544360023</v>
@@ -17584,7 +17584,7 @@
         <v>0.4982502695345901</v>
       </c>
       <c r="D539">
-        <v>1.802432891118666</v>
+        <v>1.803936203964546</v>
       </c>
       <c r="E539">
         <v>48.6653269</v>
@@ -17599,7 +17599,7 @@
         <v>0.362877749727164</v>
       </c>
       <c r="I539">
-        <v>0.6502456665039062</v>
+        <v>0.6508449912071228</v>
       </c>
       <c r="J539">
         <v>85101.74615458791</v>
@@ -17616,7 +17616,7 @@
         <v>0.5034619422573574</v>
       </c>
       <c r="D540">
-        <v>2.145063430539812</v>
+        <v>2.147256893765586</v>
       </c>
       <c r="E540">
         <v>53.02736129</v>
@@ -17631,7 +17631,7 @@
         <v>0.7700683636846728</v>
       </c>
       <c r="I540">
-        <v>0.6386415362358093</v>
+        <v>0.6392304301261902</v>
       </c>
       <c r="J540">
         <v>93812.876534775</v>
@@ -17648,7 +17648,7 @@
         <v>0.5094814150464051</v>
       </c>
       <c r="D541">
-        <v>2.140586316360153</v>
+        <v>2.142720974000468</v>
       </c>
       <c r="E541">
         <v>53.61823884</v>
@@ -17663,7 +17663,7 @@
         <v>0.1713414492450882</v>
       </c>
       <c r="I541">
-        <v>0.6292807459831238</v>
+        <v>0.6298568844795227</v>
       </c>
       <c r="J541">
         <v>94377.78991963759</v>
@@ -17680,7 +17680,7 @@
         <v>0.5108484896487172</v>
       </c>
       <c r="D542">
-        <v>2.512200364464867</v>
+        <v>2.515223878156271</v>
       </c>
       <c r="E542">
         <v>56.4754816</v>
@@ -17695,7 +17695,7 @@
         <v>1.120049613003382</v>
       </c>
       <c r="I542">
-        <v>0.6225997805595398</v>
+        <v>0.6231605410575867</v>
       </c>
       <c r="J542">
         <v>103976.137798948</v>
@@ -17712,7 +17712,7 @@
         <v>0.5113999241173621</v>
       </c>
       <c r="D543">
-        <v>2.557515312121432</v>
+        <v>2.537123351269218</v>
       </c>
       <c r="E543">
         <v>55.82312804</v>
@@ -17724,10 +17724,10 @@
         <v>1.034547608728987</v>
       </c>
       <c r="H543">
-        <v>1.28016671942206</v>
+        <v>1.479140442361926</v>
       </c>
       <c r="I543">
-        <v>0.6211040616035461</v>
+        <v>0.6216500997543335</v>
       </c>
       <c r="J543">
         <v>106015.689848919</v>
@@ -17738,31 +17738,63 @@
         <v>45796</v>
       </c>
       <c r="B544">
-        <v>2.201629677150359</v>
+        <v>2.239696187839336</v>
       </c>
       <c r="C544">
-        <v>0.5129777309146766</v>
+        <v>0.5124785202579709</v>
       </c>
       <c r="D544">
-        <v>2.582774416852897</v>
+        <v>2.627910830927721</v>
       </c>
       <c r="E544">
-        <v>56.54864012</v>
+        <v>57.54764147</v>
       </c>
       <c r="F544">
-        <v>66.07316555654444</v>
+        <v>67.40631204914088</v>
       </c>
       <c r="G544">
         <v>1.029466806382362</v>
       </c>
       <c r="H544">
-        <v>2.554532108493968</v>
+        <v>1.07694809307235</v>
       </c>
       <c r="I544">
-        <v>0.6224254369735718</v>
+        <v>0.6230008602142334</v>
       </c>
       <c r="J544">
-        <v>106662.49</v>
+        <v>108914.876558445</v>
+      </c>
+    </row>
+    <row r="545" spans="1:10">
+      <c r="A545" s="2">
+        <v>45803</v>
+      </c>
+      <c r="B545">
+        <v>2.222919334377163</v>
+      </c>
+      <c r="C545">
+        <v>0.5121196303807592</v>
+      </c>
+      <c r="D545">
+        <v>2.624038771609273</v>
+      </c>
+      <c r="E545">
+        <v>57.50215393</v>
+      </c>
+      <c r="F545">
+        <v>67.32089096633089</v>
+      </c>
+      <c r="G545">
+        <v>1.025151386750079</v>
+      </c>
+      <c r="H545">
+        <v>4.131331121446169</v>
+      </c>
+      <c r="I545">
+        <v>0.625508725643158</v>
+      </c>
+      <c r="J545">
+        <v>108847.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 6/11/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J546"/>
+  <dimension ref="A1:J547"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17776,7 +17776,7 @@
         <v>0.5128004874223953</v>
       </c>
       <c r="D545">
-        <v>2.455864361887483</v>
+        <v>2.441753621040475</v>
       </c>
       <c r="E545">
         <v>55.52576333</v>
@@ -17802,31 +17802,63 @@
         <v>45810</v>
       </c>
       <c r="B546">
-        <v>2.14215509180484</v>
+        <v>2.142933619632606</v>
       </c>
       <c r="C546">
-        <v>0.5148634938925425</v>
+        <v>0.5147901687195232</v>
       </c>
       <c r="D546">
-        <v>2.434506442617549</v>
+        <v>2.41794393107551</v>
       </c>
       <c r="E546">
-        <v>55.34293313</v>
+        <v>55.50869566</v>
       </c>
       <c r="F546">
-        <v>63.19541531327658</v>
+        <v>63.59615551936401</v>
       </c>
       <c r="G546">
         <v>1.053685673829434</v>
       </c>
       <c r="H546">
-        <v>2.860712717867298</v>
+        <v>1.514825326039593</v>
       </c>
       <c r="I546">
-        <v>0.6234190464019775</v>
+        <v>0.6233731508255005</v>
       </c>
       <c r="J546">
-        <v>105395.55</v>
+        <v>105727.739632379</v>
+      </c>
+    </row>
+    <row r="547" spans="1:10">
+      <c r="A547" s="2">
+        <v>45817</v>
+      </c>
+      <c r="B547">
+        <v>2.221509346410006</v>
+      </c>
+      <c r="C547">
+        <v>0.5162094706280251</v>
+      </c>
+      <c r="D547">
+        <v>2.591422634989009</v>
+      </c>
+      <c r="E547">
+        <v>57.12869794</v>
+      </c>
+      <c r="F547">
+        <v>66.47137797719219</v>
+      </c>
+      <c r="G547">
+        <v>1.04566606138571</v>
+      </c>
+      <c r="H547">
+        <v>1.976896779982029</v>
+      </c>
+      <c r="I547">
+        <v>0.6210340857505798</v>
+      </c>
+      <c r="J547">
+        <v>109899.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 6/18/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J547"/>
+  <dimension ref="A1:J548"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17808,7 +17808,7 @@
         <v>0.5147901687195232</v>
       </c>
       <c r="D546">
-        <v>2.41794393107551</v>
+        <v>2.403727800594599</v>
       </c>
       <c r="E546">
         <v>55.50869566</v>
@@ -17834,31 +17834,63 @@
         <v>45817</v>
       </c>
       <c r="B547">
-        <v>2.221509346410006</v>
+        <v>2.128547512337009</v>
       </c>
       <c r="C547">
-        <v>0.5162094706280251</v>
+        <v>0.5171794346541715</v>
       </c>
       <c r="D547">
-        <v>2.591422634989009</v>
+        <v>2.376987099892328</v>
       </c>
       <c r="E547">
-        <v>57.12869794</v>
+        <v>55.03723885</v>
       </c>
       <c r="F547">
-        <v>66.47137797719219</v>
+        <v>63.31637743492592</v>
       </c>
       <c r="G547">
-        <v>1.04566606138571</v>
+        <v>1.041664799124282</v>
       </c>
       <c r="H547">
-        <v>1.976896779982029</v>
+        <v>3.508037523905916</v>
       </c>
       <c r="I547">
-        <v>0.6210340857505798</v>
+        <v>0.6209878325462341</v>
       </c>
       <c r="J547">
-        <v>109899.12</v>
+        <v>105512.797437756</v>
+      </c>
+    </row>
+    <row r="548" spans="1:10">
+      <c r="A548" s="2">
+        <v>45824</v>
+      </c>
+      <c r="B548">
+        <v>2.103564244619221</v>
+      </c>
+      <c r="C548">
+        <v>0.5182071597087271</v>
+      </c>
+      <c r="D548">
+        <v>2.336227104804377</v>
+      </c>
+      <c r="E548">
+        <v>56.28200172</v>
+      </c>
+      <c r="F548">
+        <v>61.95536543566842</v>
+      </c>
+      <c r="G548">
+        <v>1.035501376716595</v>
+      </c>
+      <c r="H548">
+        <v>0.4970138481538378</v>
+      </c>
+      <c r="I548">
+        <v>0.6180257201194763</v>
+      </c>
+      <c r="J548">
+        <v>104516.16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
weekly update eclipse 6/25/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J548"/>
+  <dimension ref="A1:J549"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -17840,7 +17840,7 @@
         <v>0.5171794346541715</v>
       </c>
       <c r="D547">
-        <v>2.376987099892328</v>
+        <v>2.364345730522425</v>
       </c>
       <c r="E547">
         <v>55.03723885</v>
@@ -17866,31 +17866,63 @@
         <v>45824</v>
       </c>
       <c r="B548">
-        <v>2.103564244619221</v>
+        <v>2.026386313165476</v>
       </c>
       <c r="C548">
-        <v>0.5182071597087271</v>
+        <v>0.5190093422539663</v>
       </c>
       <c r="D548">
-        <v>2.336227104804377</v>
+        <v>2.163144606574715</v>
       </c>
       <c r="E548">
-        <v>56.28200172</v>
+        <v>53.10243876</v>
       </c>
       <c r="F548">
-        <v>61.95536543566842</v>
+        <v>57.47199545714039</v>
       </c>
       <c r="G548">
         <v>1.035501376716595</v>
       </c>
       <c r="H548">
-        <v>0.4970138481538378</v>
+        <v>1.151974965899605</v>
       </c>
       <c r="I548">
-        <v>0.6180257201194763</v>
+        <v>0.6179842352867126</v>
       </c>
       <c r="J548">
-        <v>104516.16</v>
+        <v>100899.234151958</v>
+      </c>
+    </row>
+    <row r="549" spans="1:10">
+      <c r="A549" s="2">
+        <v>45831</v>
+      </c>
+      <c r="B549">
+        <v>2.121635817703177</v>
+      </c>
+      <c r="C549">
+        <v>0.5193753003842977</v>
+      </c>
+      <c r="D549">
+        <v>2.363566618697726</v>
+      </c>
+      <c r="E549">
+        <v>54.00293061</v>
+      </c>
+      <c r="F549">
+        <v>61.66076112369596</v>
+      </c>
+      <c r="G549">
+        <v>1.030276201921373</v>
+      </c>
+      <c r="H549">
+        <v>1.859693953043351</v>
+      </c>
+      <c r="I549">
+        <v>0.6101500391960144</v>
+      </c>
+      <c r="J549">
+        <v>105969.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 7/30/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J553"/>
+  <dimension ref="A1:J554"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18000,7 +18000,7 @@
         <v>0.5134785305661046</v>
       </c>
       <c r="D552">
-        <v>2.608011150417588</v>
+        <v>2.600957314507738</v>
       </c>
       <c r="E552">
         <v>57.08653384</v>
@@ -18026,31 +18026,63 @@
         <v>45859</v>
       </c>
       <c r="B553">
-        <v>2.150095356362578</v>
+        <v>2.195359213879629</v>
       </c>
       <c r="C553">
-        <v>0.5077764318612117</v>
+        <v>0.5073202716351362</v>
       </c>
       <c r="D553">
-        <v>2.596509355773671</v>
+        <v>2.654884034343522</v>
       </c>
       <c r="E553">
-        <v>56.98064572</v>
+        <v>56.75465963</v>
       </c>
       <c r="F553">
-        <v>67.9209553293008</v>
+        <v>69.3472186040632</v>
       </c>
       <c r="G553">
-        <v>1.028476495728439</v>
+        <v>1.037833862252505</v>
       </c>
       <c r="H553">
-        <v>1.642734467635432</v>
+        <v>1.663718955694704</v>
       </c>
       <c r="I553">
-        <v>0.6132335066795349</v>
+        <v>0.6132102012634277</v>
       </c>
       <c r="J553">
-        <v>117206.16</v>
+        <v>119438.164235535</v>
+      </c>
+    </row>
+    <row r="554" spans="1:10">
+      <c r="A554" s="2">
+        <v>45866</v>
+      </c>
+      <c r="B554">
+        <v>2.151449607815851</v>
+      </c>
+      <c r="C554">
+        <v>0.5019386663414789</v>
+      </c>
+      <c r="D554">
+        <v>2.588334070386426</v>
+      </c>
+      <c r="E554">
+        <v>56.66310363</v>
+      </c>
+      <c r="F554">
+        <v>66.94028694179676</v>
+      </c>
+      <c r="G554">
+        <v>1.032254693412495</v>
+      </c>
+      <c r="H554">
+        <v>2.693439234908368</v>
+      </c>
+      <c r="I554">
+        <v>0.6170766949653625</v>
+      </c>
+      <c r="J554">
+        <v>117678.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 6/8/25
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J554"/>
+  <dimension ref="A1:J555"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18032,7 +18032,7 @@
         <v>0.5073202716351362</v>
       </c>
       <c r="D553">
-        <v>2.654884034343522</v>
+        <v>2.638712204040376</v>
       </c>
       <c r="E553">
         <v>56.75465963</v>
@@ -18058,31 +18058,63 @@
         <v>45866</v>
       </c>
       <c r="B554">
-        <v>2.151449607815851</v>
+        <v>2.086229037097489</v>
       </c>
       <c r="C554">
-        <v>0.5019386663414789</v>
+        <v>0.5026157914323811</v>
       </c>
       <c r="D554">
-        <v>2.588334070386426</v>
+        <v>2.421640412293536</v>
       </c>
       <c r="E554">
-        <v>56.66310363</v>
+        <v>54.50458753</v>
       </c>
       <c r="F554">
-        <v>66.94028694179676</v>
+        <v>62.71593521981282</v>
       </c>
       <c r="G554">
         <v>1.032254693412495</v>
       </c>
       <c r="H554">
-        <v>2.693439234908368</v>
+        <v>0.8136597326489525</v>
       </c>
       <c r="I554">
-        <v>0.6170766949653625</v>
+        <v>0.6170238852500916</v>
       </c>
       <c r="J554">
-        <v>117678.53</v>
+        <v>114263.693947691</v>
+      </c>
+    </row>
+    <row r="555" spans="1:10">
+      <c r="A555" s="2">
+        <v>45873</v>
+      </c>
+      <c r="B555">
+        <v>2.065270235834697</v>
+      </c>
+      <c r="C555">
+        <v>0.498657537910168</v>
+      </c>
+      <c r="D555">
+        <v>2.413008708180225</v>
+      </c>
+      <c r="E555">
+        <v>55.32385364</v>
+      </c>
+      <c r="F555">
+        <v>61.77117994256373</v>
+      </c>
+      <c r="G555">
+        <v>1.027520072709576</v>
+      </c>
+      <c r="H555">
+        <v>1.033137719867661</v>
+      </c>
+      <c r="I555">
+        <v>0.6164847612380981</v>
+      </c>
+      <c r="J555">
+        <v>113495.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Weekly update eclipse 8/13
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J555"/>
+  <dimension ref="A1:J556"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18064,7 +18064,7 @@
         <v>0.5026157914323811</v>
       </c>
       <c r="D554">
-        <v>2.421640412293536</v>
+        <v>2.406494895116896</v>
       </c>
       <c r="E554">
         <v>54.50458753</v>
@@ -18090,31 +18090,63 @@
         <v>45873</v>
       </c>
       <c r="B555">
-        <v>2.065270235834697</v>
+        <v>2.164097282715636</v>
       </c>
       <c r="C555">
-        <v>0.498657537910168</v>
+        <v>0.4975558624398717</v>
       </c>
       <c r="D555">
-        <v>2.413008708180225</v>
+        <v>2.577942113547076</v>
       </c>
       <c r="E555">
-        <v>55.32385364</v>
+        <v>55.66488389</v>
       </c>
       <c r="F555">
-        <v>61.77117994256373</v>
+        <v>66.0444381409975</v>
       </c>
       <c r="G555">
-        <v>1.027520072709576</v>
+        <v>1.039963338485894</v>
       </c>
       <c r="H555">
-        <v>1.033137719867661</v>
+        <v>1.454310937743797</v>
       </c>
       <c r="I555">
-        <v>0.6164847612380981</v>
+        <v>0.6164355278015137</v>
       </c>
       <c r="J555">
-        <v>113495.19</v>
+        <v>119189.198160275</v>
+      </c>
+    </row>
+    <row r="556" spans="1:10">
+      <c r="A556" s="2">
+        <v>45880</v>
+      </c>
+      <c r="B556">
+        <v>2.17317082318996</v>
+      </c>
+      <c r="C556">
+        <v>0.4913861157764893</v>
+      </c>
+      <c r="D556">
+        <v>2.610263637128486</v>
+      </c>
+      <c r="E556">
+        <v>56.40376131</v>
+      </c>
+      <c r="F556">
+        <v>66.5734442359656</v>
+      </c>
+      <c r="G556">
+        <v>1.034059840852372</v>
+      </c>
+      <c r="H556">
+        <v>1.454768189720923</v>
+      </c>
+      <c r="I556">
+        <v>0.6161071062088013</v>
+      </c>
+      <c r="J556">
+        <v>119999.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour automatique des fichiers Eclipse Replication
</commit_message>
<xml_diff>
--- a/static/assets/LastUpdatedWithPredictions.xlsx
+++ b/static/assets/LastUpdatedWithPredictions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="525">
   <si>
     <t>date</t>
   </si>
@@ -1586,6 +1586,9 @@
   </si>
   <si>
     <t>2025-11-03</t>
+  </si>
+  <si>
+    <t>2025-11-10</t>
   </si>
 </sst>
 </file>
@@ -1943,7 +1946,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J515"/>
+  <dimension ref="A1:J516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -18402,7 +18405,7 @@
         <v>523</v>
       </c>
       <c r="B515">
-        <v>1.662703831034413</v>
+        <v>1.701221501440441</v>
       </c>
       <c r="C515">
         <v>0.4833874244237868</v>
@@ -18414,19 +18417,51 @@
         <v>104685.54544097</v>
       </c>
       <c r="F515">
-        <v>1.6266</v>
+        <v>1.6571</v>
       </c>
       <c r="G515">
-        <v>45.7259574</v>
+        <v>46.36746156</v>
       </c>
       <c r="H515">
         <v>1.08222548465759</v>
       </c>
       <c r="I515">
-        <v>0.6005020203657896</v>
+        <v>0.3742016676881788</v>
       </c>
       <c r="J515">
         <v>0.557752788066864</v>
+      </c>
+    </row>
+    <row r="516" spans="1:10">
+      <c r="A516" t="s">
+        <v>524</v>
+      </c>
+      <c r="B516">
+        <v>1.669450381830717</v>
+      </c>
+      <c r="C516">
+        <v>0.4871634535204017</v>
+      </c>
+      <c r="D516">
+        <v>45.29370825428658</v>
+      </c>
+      <c r="E516">
+        <v>102988.81</v>
+      </c>
+      <c r="F516">
+        <v>1.7319</v>
+      </c>
+      <c r="G516">
+        <v>45.41554149</v>
+      </c>
+      <c r="H516">
+        <v>1.069660717385277</v>
+      </c>
+      <c r="I516">
+        <v>0.4081487342959988</v>
+      </c>
+      <c r="J516">
+        <v>0.5437155365943909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>